<commit_message>
trying to fix the reference file
</commit_message>
<xml_diff>
--- a/paper/duplicates excel.xlsx
+++ b/paper/duplicates excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/Outliers/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44493415-D154-184F-A50F-6791AABA42C9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EADD366E-33F6-DB4B-BE02-C44317E8FC21}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{64E93A58-47E1-B74E-9896-FCF6FAC1E62F}"/>
   </bookViews>
@@ -13156,7 +13156,7 @@
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -13182,24 +13182,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -52580,8 +52562,8 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>